<commit_message>
Criou o script R diagrama_linha_orçamento_justiça_2010_2025
</commit_message>
<xml_diff>
--- a/analise-dados/orçamento_justiça_2010_2025.xlsx
+++ b/analise-dados/orçamento_justiça_2010_2025.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Master-Dissertation\analise-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6715FB3-2973-4613-A87F-9A5399928990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8968C8-005E-42D5-9F56-326A690ADC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CNJ</t>
   </si>
@@ -118,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,27 +132,43 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,16 +176,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -468,659 +503,603 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>510935728</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>503017061</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>525207236</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="6">
         <v>519810690</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="7">
         <v>564146036</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="8">
         <v>603855678</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="8">
         <v>554750410</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="8">
         <v>686232270</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="8">
         <v>714059827</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="8">
         <v>778625817</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="8">
         <v>686719630</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="8">
         <v>712462432</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="8">
         <v>761903593</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="8">
         <v>851741456</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="9">
         <v>897618717</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="9">
         <v>953887705</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>886662747</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>942244077</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>964712754</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6">
         <v>1023485635</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="7">
         <v>1133154967</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="8">
         <v>1301664660</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="8">
         <v>1164743540</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="8">
         <v>1418469714</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="8">
         <v>1536877868</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="8">
         <v>1644751462</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="8">
         <v>1625723822</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="8">
         <v>1684375322</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="8">
         <v>1809298602</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="8">
         <v>2029721389</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="9">
         <v>2104718497</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="9">
         <v>2247534274</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>6778113997</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>6917433514</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>7279847920</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <v>7764040936</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="7">
         <v>8998633172</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="8">
         <v>10192650978</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="8">
         <v>9797077381</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="8">
         <v>11582502711</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="8">
         <v>11966883055</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="8">
         <v>12855991338</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="8">
         <v>12323121522</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="8">
         <v>12956342248</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="8">
         <v>13925921922</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="8">
         <v>15477560643</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="9">
         <v>16156788503</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="9">
         <v>17214461661</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>349488205</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>361136340</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>388205646</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>429741527</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="7">
         <v>434709854</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="8">
         <v>464278536</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="8">
         <v>436744289</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="8">
         <v>530823790</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="8">
         <v>550051578</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="8">
         <v>593613268</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="8">
         <v>580749627</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="8">
         <v>597937112</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="8">
         <v>643078345</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="8">
         <v>722362628</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="9">
         <v>758713265</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="9">
         <v>803257033</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>5205604298</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>4496352698</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>5398864227</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>4954842604</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="7">
         <v>6077120836</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="8">
         <v>6564757818</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>6846524634</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="8">
         <v>7739630644</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="8">
         <v>8928427580</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="8">
         <v>8603604228</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="8">
         <v>9274591509</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="8">
         <v>9472037516</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="8">
         <v>10281590553</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="8">
         <v>10678418249</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="9">
         <v>11806931675</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="9">
         <v>11298228878</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>11872611818</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>12418732769</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>13525956290</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>14358172411</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="7">
         <v>15410737549</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="8">
         <v>16676696355</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>17126685840</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="8">
         <v>20133813958</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="8">
         <v>20903063300</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="8">
         <v>22184838196</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="8">
         <v>20806855284</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="8">
         <v>21799557776</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="8">
         <v>23365981352</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="8">
         <v>26045936890</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="9">
         <v>26974930581</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="9">
         <v>30479055568</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>1558244460</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>1641510338</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>1756308454</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <v>1795306398</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="7">
         <v>2020784552</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="8">
         <v>2295592718</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="4">
         <v>2294628268</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="8">
         <v>2715292874</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="8">
         <v>2812916275</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="8">
         <v>3013451132</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="8">
         <v>2955719985</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="8">
         <v>3087564524</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="8">
         <v>3307742153</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="8">
         <v>3708490346</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="9">
         <v>3844766122</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="9">
         <v>4083171539</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>193065544</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>195312144</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>235842984</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>232565685</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="7">
         <v>219262114</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="6">
         <v>285360365</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>218952516</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="8">
         <v>223593294</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="8">
         <v>220770001</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="8">
         <v>231178608</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="8">
         <v>205311608</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="8">
         <v>211458134</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="8">
         <v>228306838</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="8">
         <v>255251629</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="9">
         <v>297751922</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="9">
         <v>318967069</v>
       </c>
     </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H6:H9">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359EB966-33B6-48F1-A39E-A9ED60D6B0AC}">
-  <dimension ref="A1:Q9"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:Q9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="4" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1">
-        <v>2010</v>
-      </c>
-      <c r="C1">
-        <v>2011</v>
-      </c>
-      <c r="D1">
-        <v>2012</v>
-      </c>
-      <c r="E1">
-        <v>2013</v>
-      </c>
-      <c r="F1">
-        <v>2014</v>
-      </c>
-      <c r="G1">
-        <v>2015</v>
-      </c>
-      <c r="H1">
-        <v>2016</v>
-      </c>
-      <c r="I1">
-        <v>2017</v>
-      </c>
-      <c r="J1">
-        <v>2018</v>
-      </c>
-      <c r="K1">
-        <v>2019</v>
-      </c>
-      <c r="L1">
-        <v>2020</v>
-      </c>
-      <c r="M1">
-        <v>2021</v>
-      </c>
-      <c r="N1">
-        <v>2022</v>
-      </c>
-      <c r="O1">
-        <v>2023</v>
-      </c>
-      <c r="P1">
-        <v>2024</v>
-      </c>
-      <c r="Q1">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>510935728</v>
-      </c>
-      <c r="C2" s="4">
-        <v>503017061</v>
-      </c>
-      <c r="D2" s="4">
-        <v>525207236</v>
-      </c>
-      <c r="E2" s="1">
-        <v>519810690</v>
-      </c>
-      <c r="F2" s="3">
-        <v>564146036</v>
-      </c>
-      <c r="G2" s="2">
-        <v>603855678</v>
-      </c>
-      <c r="H2" s="2">
-        <v>554750410</v>
-      </c>
-      <c r="I2" s="2">
-        <v>686232270</v>
-      </c>
-      <c r="J2" s="2">
-        <v>714059827</v>
-      </c>
-      <c r="K2" s="2">
-        <v>778625817</v>
-      </c>
-      <c r="L2" s="2">
-        <v>686719630</v>
-      </c>
-      <c r="M2" s="2">
-        <v>712462432</v>
-      </c>
-      <c r="N2" s="2">
-        <v>761903593</v>
-      </c>
-      <c r="O2" s="2">
-        <v>851741456</v>
-      </c>
-      <c r="P2" s="2">
-        <v>897618717</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>953887705</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removeu a extensão dos scripts para transformá-los em notebooks Python
</commit_message>
<xml_diff>
--- a/analise-dados/orçamento_justiça_2010_2025.xlsx
+++ b/analise-dados/orçamento_justiça_2010_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Master-Dissertation\analise-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8968C8-005E-42D5-9F56-326A690ADC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076122D5-505D-44F8-87BB-A7C57D047ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CNJ</t>
   </si>
@@ -63,54 +63,6 @@
   </si>
   <si>
     <t>Orgao</t>
-  </si>
-  <si>
-    <t>A2010</t>
-  </si>
-  <si>
-    <t>A2011</t>
-  </si>
-  <si>
-    <t>A2012</t>
-  </si>
-  <si>
-    <t>A2013</t>
-  </si>
-  <si>
-    <t>A2014</t>
-  </si>
-  <si>
-    <t>A2015</t>
-  </si>
-  <si>
-    <t>A2016</t>
-  </si>
-  <si>
-    <t>A2017</t>
-  </si>
-  <si>
-    <t>A2018</t>
-  </si>
-  <si>
-    <t>A2019</t>
-  </si>
-  <si>
-    <t>A2020</t>
-  </si>
-  <si>
-    <t>A2021</t>
-  </si>
-  <si>
-    <t>A2022</t>
-  </si>
-  <si>
-    <t>A2023</t>
-  </si>
-  <si>
-    <t>A2024</t>
-  </si>
-  <si>
-    <t>A2025</t>
   </si>
 </sst>
 </file>
@@ -489,7 +441,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -506,53 +458,53 @@
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>24</v>
+      <c r="B1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="L1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="M1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2022</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2023</v>
+      </c>
+      <c r="P1" s="3">
+        <v>2024</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>2025</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>